<commit_message>
12.03 SRS 1.2 수정
</commit_message>
<xml_diff>
--- a/Test/Test Case_Test Result.xlsx
+++ b/Test/Test Case_Test Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\filling-good\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47716CCC-0963-4274-A659-77C1A23BEADA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BFD8E5-BE32-4BF1-99C4-E13A5D946A8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario_with _BF" sheetId="1" r:id="rId1"/>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1290,7 +1290,7 @@
   <dimension ref="B3:J15"/>
   <sheetViews>
     <sheetView zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1651,7 +1651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E278BB-833E-405A-8CA5-8894D0B1DE9D}">
   <dimension ref="B3:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
12.05 Test case 수정
</commit_message>
<xml_diff>
--- a/Test/Test Case_Test Result.xlsx
+++ b/Test/Test Case_Test Result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\filling-good\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138B435D-6DFF-4820-9C2F-891D4E2EAFB3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6544D5F4-D8A6-4002-B0DD-87B2ACA6F86E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20310" windowHeight="16110" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario_with _BF" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="162">
   <si>
     <t>Basic Flow #</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -471,10 +471,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AF3. 시간/장소 피드백이 변하지 않은 경우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TC_37</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -511,14 +507,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AF4. 가중치 범위를 벗어난 경우(시간대 가중치 최대치)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AF4. 가중치 범위를 벗어난 경우(일정 조정 가중치 최소치)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>피드백 생성(좋음,나쁨), 겹치는 일정 있는 경우</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -527,38 +515,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>일정의 조정 가중치 감소, 장소 우선순위 증가하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일정의 조정 가중치 최소치, 장소 우선순위 증가하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간대 가중치 증가, 장소 우선순위 증가하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간대 가중치 최대치, 장소 우선순위 증가하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일정의 조정 가중치 감소, 장소 우선순위 감소하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일정의 조정 가중치 최소치, 장소 우선순위 감소하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간대 가중치 증가, 장소 우선순위 감소하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간대 가중치 최대치, 장소 우선순위 감소하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>피드백 생성(나쁨,좋음), 겹치는 일정 있는 경우</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -567,51 +523,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AF4. 가중치 범위를 벗어난 경우(일정 조정 가중치 최대치)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AF4. 가중치 범위를 벗어난 경우(시간대 가중치 최소치)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일정의 조정 가중치 증가, 장소 우선순위 증가하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일정의 조정 가중치 최대치, 장소 우선순위 증가하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간대 가중치 최소치, 장소 우선순위 증가하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간대 가중치 감소, 장소 우선순위 증가하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>피드백 생성(나쁨,나쁨), 겹치는 일정 있는 경우</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>피드백 생성(나쁨,나쁨), 겹치는 일정 없는 경우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일정의 조정 가중치 증가, 장소 우선순위 감소하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일정의 조정 가중치 최대치, 장소 우선순위 감소하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간대 가중치 감소, 장소 우선순위 감소하며 새로운 피드백 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간대 가중치 최소치, 장소 우선순위 감소하며 새로운 피드백 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -840,6 +756,115 @@
     <t>모임 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>일정의 조정 가중치 감소, 장소 우선순위 
+증가하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피드백 생성(좋음,나쁨), 겹치는 일정없는 경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정의 조정 가중치 최소치, 장소 우선순위
+ 증가하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대 가중치 증가, 장소 우선순위
+ 증가하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대 가중치 최대치, 장소 우선순위
+ 증가하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정의 조정 가중치 감소, 장소 우선순위 
+감소하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정의 조정 가중치 최소치, 장소 우선순위 
+감소하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대 가중치 증가, 장소 우선순위 
+감소하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대 가중치 최대치, 장소 우선순위 
+감소하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정의 조정 가중치 증가, 장소 우선순위 
+증가하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정의 조정 가중치 최대치, 장소 우선순위
+ 증가하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대 가중치 감소, 장소 우선순위 
+증가하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대 가중치 최소치, 장소 우선순위 
+증가하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정의 조정 가중치 증가, 장소 우선순위 
+감소하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정의 조정 가중치 최대치, 장소 우선순위
+ 감소하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대 가중치 감소, 장소 우선순위 
+감소하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대 가중치 최소치, 장소 우선순위 
+감소하며 새로운 피드백 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AF4. 가중치 범위를 벗어난 경우
+(일정 조정 가중치 최소치)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AF4. 가중치 범위를 벗어난 경우
+(시간대 가중치 최대치)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AF4. 가중치 범위를 벗어난 경우
+(일정 조정 가중치 최대치)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AF4. 가중치 범위를 벗어난 경우
+(시간대 가중치 최소치)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AF3. 시간/장소 피드백이 변하지 
+않은 경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -897,7 +922,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -944,11 +969,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -984,9 +1033,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,6 +1053,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1294,17 +1349,17 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.125" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="36.125" customWidth="1"/>
-    <col min="6" max="6" width="35.625" customWidth="1"/>
-    <col min="7" max="7" width="32.75" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.09765625" customWidth="1"/>
+    <col min="4" max="4" width="17.19921875" customWidth="1"/>
+    <col min="5" max="5" width="36.09765625" customWidth="1"/>
+    <col min="6" max="6" width="35.59765625" customWidth="1"/>
+    <col min="7" max="7" width="32.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1324,7 +1379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1347,7 +1402,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1361,7 +1416,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1375,7 +1430,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
@@ -1389,7 +1444,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" s="2" t="s">
         <v>48</v>
       </c>
@@ -1403,7 +1458,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1411,7 +1466,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1419,7 +1474,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1427,7 +1482,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1435,7 +1490,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1443,7 +1498,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1451,7 +1506,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1459,7 +1514,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1478,24 +1533,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:J19"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A8" zoomScale="80" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.125" customWidth="1"/>
-    <col min="4" max="4" width="20.25" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.75" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.09765625" customWidth="1"/>
+    <col min="4" max="4" width="20.19921875" customWidth="1"/>
+    <col min="5" max="5" width="17.59765625" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.69921875" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="19.625" customWidth="1"/>
-    <col min="10" max="10" width="9.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.59765625" customWidth="1"/>
+    <col min="10" max="10" width="9.19921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1524,7 +1579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
@@ -1547,7 +1602,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1572,7 +1627,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1595,7 +1650,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
@@ -1620,7 +1675,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
@@ -1645,7 +1700,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
@@ -1670,7 +1725,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
@@ -1695,7 +1750,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
@@ -1718,7 +1773,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
@@ -1743,7 +1798,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B13" s="4" t="s">
         <v>44</v>
       </c>
@@ -1768,7 +1823,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B14" s="4" t="s">
         <v>44</v>
       </c>
@@ -1793,7 +1848,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
@@ -1818,7 +1873,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B16" s="4" t="s">
         <v>48</v>
       </c>
@@ -1841,7 +1896,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
@@ -1866,12 +1921,12 @@
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B18"/>
       <c r="F18"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B19"/>
       <c r="F19"/>
       <c r="J19"/>
@@ -1885,26 +1940,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5834CD0C-44D3-4F89-9ED5-7369E7AB8B68}">
-  <dimension ref="B3:J15"/>
+  <dimension ref="B3:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.125" customWidth="1"/>
-    <col min="4" max="4" width="20.25" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.75" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.09765625" customWidth="1"/>
+    <col min="4" max="4" width="20.19921875" customWidth="1"/>
+    <col min="5" max="5" width="17.59765625" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.69921875" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="19.625" customWidth="1"/>
-    <col min="10" max="10" width="9.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.59765625" customWidth="1"/>
+    <col min="10" max="10" width="9.19921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1933,225 +1988,203 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B4" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14" t="s">
+      <c r="D4" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B5" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B6" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B7" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B8" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B9" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B10" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="G10" s="14"/>
+      <c r="H10" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B11" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="17" t="s">
+      <c r="D11" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="F11" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="G11" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="14" t="s">
+      <c r="H11" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="14"/>
-    </row>
-    <row r="8" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="2:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14"/>
-      <c r="F14"/>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15"/>
-      <c r="F15"/>
-      <c r="J15"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B12"/>
+      <c r="F12"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B13"/>
+      <c r="F13"/>
+      <c r="J13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2168,20 +2201,20 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.125" customWidth="1"/>
-    <col min="4" max="4" width="20.25" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.75" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.09765625" customWidth="1"/>
+    <col min="4" max="4" width="20.19921875" customWidth="1"/>
+    <col min="5" max="5" width="17.59765625" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.69921875" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="19.625" customWidth="1"/>
-    <col min="10" max="10" width="9.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.59765625" customWidth="1"/>
+    <col min="10" max="10" width="9.19921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2210,7 +2243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>67</v>
       </c>
@@ -2227,7 +2260,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2238,7 +2271,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2249,7 +2282,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2260,7 +2293,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2271,7 +2304,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -2282,7 +2315,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2293,7 +2326,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2304,7 +2337,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2315,7 +2348,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2326,12 +2359,12 @@
       <c r="I13" s="5"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B14"/>
       <c r="F14"/>
       <c r="J14"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B15"/>
       <c r="F15"/>
       <c r="J15"/>
@@ -2345,27 +2378,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E278BB-833E-405A-8CA5-8894D0B1DE9D}">
-  <dimension ref="B3:J30"/>
+  <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.75" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.75" customWidth="1"/>
-    <col min="4" max="4" width="20.25" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.75" customWidth="1"/>
-    <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="19.625" customWidth="1"/>
-    <col min="10" max="10" width="9.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.69921875" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="40.19921875" customWidth="1"/>
+    <col min="5" max="5" width="31.296875" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.69921875" customWidth="1"/>
+    <col min="8" max="8" width="36.3984375" customWidth="1"/>
+    <col min="9" max="9" width="27.09765625" customWidth="1"/>
+    <col min="10" max="10" width="9.19921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2394,30 +2430,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>76</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="I4" s="5"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B5" s="4" t="s">
         <v>79</v>
       </c>
@@ -2425,7 +2461,7 @@
         <v>65</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>85</v>
@@ -2435,364 +2471,364 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B6" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2" t="s">
+      <c r="D6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B7" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2" t="s">
+      <c r="D8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B9" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="D9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B10" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2" t="s">
+      <c r="D10" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>112</v>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B11" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="D11" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>113</v>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B12" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2" t="s">
+      <c r="D12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>114</v>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B13" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="D13" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>115</v>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B14" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2" t="s">
+      <c r="D14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
-        <v>120</v>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+    <row r="15" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B15" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="D15" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>121</v>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B16" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2" t="s">
+      <c r="D16" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3" t="s">
-        <v>123</v>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B17" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="D17" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3" t="s">
-        <v>122</v>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
+    <row r="18" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B18" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2" t="s">
+      <c r="D18" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
+      <c r="G18" s="5"/>
+      <c r="H18" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B19" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="D19" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="G19" s="5"/>
+      <c r="H19" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B20" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2" t="s">
+      <c r="D20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+      <c r="G20" s="5"/>
+      <c r="H20" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B21" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="D21" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G21" s="5"/>
+      <c r="H21" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2803,7 +2839,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B23" s="4" t="s">
         <v>88</v>
       </c>
@@ -2811,7 +2847,7 @@
         <v>65</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="4" t="s">
@@ -2824,30 +2860,30 @@
       <c r="I23" s="5"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B24" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="D24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B25" s="4" t="s">
         <v>93</v>
       </c>
@@ -2855,44 +2891,45 @@
         <v>65</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B26" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>85</v>
       </c>
       <c r="F26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B27" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>65</v>
@@ -2902,9 +2939,10 @@
       <c r="F27" s="4"/>
       <c r="G27" s="9"/>
       <c r="H27" s="5"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I27" s="21"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -2912,12 +2950,14 @@
       <c r="F28" s="4"/>
       <c r="G28" s="9"/>
       <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I28" s="22"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B29"/>
       <c r="F29"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B30"/>
       <c r="F30"/>
     </row>

</xml_diff>

<commit_message>
12.06 SRS 1.3 수정
</commit_message>
<xml_diff>
--- a/Test/Test Case_Test Result.xlsx
+++ b/Test/Test Case_Test Result.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\filling-good\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AFA02B-C881-47BF-97DF-D85185F6BAB6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F60C1FB-7A65-4B65-9AC1-64698868222C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario_with _BF" sheetId="1" r:id="rId1"/>
-    <sheet name="개인일정관리" sheetId="2" r:id="rId2"/>
-    <sheet name="모임그룹관리" sheetId="5" r:id="rId3"/>
-    <sheet name="모임 장소 및 시간 추천" sheetId="6" r:id="rId4"/>
-    <sheet name="추천 모임일정에 대한 피드백" sheetId="7" r:id="rId5"/>
+    <sheet name="UC1-개인일정관리" sheetId="2" r:id="rId2"/>
+    <sheet name="UC2-모임그룹관리" sheetId="5" r:id="rId3"/>
+    <sheet name="UC3-모임 장소 및 시간 추천" sheetId="6" r:id="rId4"/>
+    <sheet name="UC4-추천 모임일정에 대한 피드백" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="165">
   <si>
     <t>Basic Flow #</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -586,11 +586,6 @@
     <t>TC_16</t>
   </si>
   <si>
-    <t>모임 수정' 버튼 클릭 후, “모임 정보를 수정하시겠습니까?”라는 메시지의
-'취소' 버튼 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> 수정된 모임 정보를 저장하지 않고 본 유스케이스를 종료</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -605,13 +600,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SC_18</t>
-  </si>
-  <si>
     <t>AF4. 모임 삭제 취소</t>
-  </si>
-  <si>
-    <t>TC_18</t>
   </si>
   <si>
     <t>모임 삭제' 버튼 클릭 후, “모임을 삭제하시겠습니까?”라는 메시지의
@@ -754,6 +743,34 @@
       </rPr>
       <t>’라는 메세지를 화면상출력</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모임 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AF2. 변경 권한 없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모임 수정' 버튼 클릭 후, “모임 정보를 수정하시겠습니까?”라는 메시지의 '취소' 버튼 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_19</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1428,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1835,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5834CD0C-44D3-4F89-9ED5-7369E7AB8B68}">
-  <dimension ref="B3:J13"/>
+  <dimension ref="B3:J14"/>
   <sheetViews>
-    <sheetView zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1891,7 +1908,7 @@
         <v>61</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="13" t="s">
@@ -1912,7 +1929,7 @@
         <v>61</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>111</v>
@@ -1937,7 +1954,7 @@
         <v>61</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="13" t="s">
@@ -1958,7 +1975,7 @@
         <v>61</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>111</v>
@@ -1983,7 +2000,7 @@
         <v>61</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>120</v>
@@ -1995,7 +2012,7 @@
         <v>122</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="13"/>
@@ -2008,7 +2025,7 @@
         <v>61</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>124</v>
@@ -2017,69 +2034,94 @@
         <v>125</v>
       </c>
       <c r="G9" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H9" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>127</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B10" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B11" s="13" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>61</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>132</v>
+        <v>160</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>135</v>
+        <v>162</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>157</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B12"/>
-      <c r="F12"/>
-      <c r="J12"/>
+    <row r="12" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B12" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B13"/>
       <c r="F13"/>
       <c r="J13"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B14"/>
+      <c r="F14"/>
+      <c r="J14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2093,7 +2135,7 @@
   <dimension ref="B3:J15"/>
   <sheetViews>
     <sheetView zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2275,8 +2317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E278BB-833E-405A-8CA5-8894D0B1DE9D}">
   <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A12" zoomScale="76" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2387,7 +2429,7 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="4"/>
@@ -2403,14 +2445,14 @@
         <v>100</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="4"/>
@@ -2431,7 +2473,7 @@
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2447,14 +2489,14 @@
         <v>101</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="4"/>
@@ -2475,7 +2517,7 @@
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="4"/>
@@ -2491,14 +2533,14 @@
         <v>102</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>85</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4"/>
@@ -2519,7 +2561,7 @@
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="4"/>
@@ -2532,17 +2574,17 @@
         <v>64</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="4"/>
@@ -2563,7 +2605,7 @@
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="4"/>
@@ -2579,14 +2621,14 @@
         <v>104</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>85</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
@@ -2607,7 +2649,7 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="4"/>
@@ -2623,14 +2665,14 @@
         <v>105</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>85</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
@@ -2651,7 +2693,7 @@
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="4"/>
@@ -2667,14 +2709,14 @@
         <v>106</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="4"/>
@@ -2695,7 +2737,7 @@
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="4"/>
@@ -2711,14 +2753,14 @@
         <v>107</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="4"/>
@@ -2766,7 +2808,7 @@
         <v>108</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>91</v>

</xml_diff>